<commit_message>
doing checks on oneOf fields
</commit_message>
<xml_diff>
--- a/datasheets/CINECA_synthetic_cohort_EUROPE_UK1.xlsx
+++ b/datasheets/CINECA_synthetic_cohort_EUROPE_UK1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oriol/Desktop/beacon-ri-tools-v2/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9DCAB5-E67B-4142-B4D5-6E2A64DC1488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFCB57E-F57D-084D-81B5-B0ABB9D96831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7920" yWindow="860" windowWidth="28040" windowHeight="16280" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="analyses" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="410">
   <si>
     <t>aligner</t>
   </si>
@@ -850,60 +850,60 @@
     <t>variation|location|_id</t>
   </si>
   <si>
+    <t>variation|location|chr</t>
+  </si>
+  <si>
+    <t>variation|location|interval</t>
+  </si>
+  <si>
+    <t>variation|location|interval|end</t>
+  </si>
+  <si>
+    <t>variation|location|interval|end|comparator</t>
+  </si>
+  <si>
+    <t>variation|location|interval|end|max</t>
+  </si>
+  <si>
+    <t>variation|location|interval|end|min</t>
+  </si>
+  <si>
+    <t>variation|location|interval|end|type</t>
+  </si>
+  <si>
+    <t>variation|location|interval|end|value</t>
+  </si>
+  <si>
+    <t>variation|location|interval|start</t>
+  </si>
+  <si>
+    <t>variation|location|interval|start|comparator</t>
+  </si>
+  <si>
+    <t>variation|location|interval|start|max</t>
+  </si>
+  <si>
+    <t>variation|location|interval|start|min</t>
+  </si>
+  <si>
+    <t>variation|location|interval|start|type</t>
+  </si>
+  <si>
+    <t>variation|location|interval|start|value</t>
+  </si>
+  <si>
+    <t>variation|location|interval|type</t>
+  </si>
+  <si>
+    <t>variation|location|sequence_id</t>
+  </si>
+  <si>
+    <t>variation|location|species_id</t>
+  </si>
+  <si>
     <t>variation|location|type</t>
   </si>
   <si>
-    <t>variation|location|species_id</t>
-  </si>
-  <si>
-    <t>variation|location|chr</t>
-  </si>
-  <si>
-    <t>variation|location|interval</t>
-  </si>
-  <si>
-    <t>variation|location|sequence_id</t>
-  </si>
-  <si>
-    <t>variation|location|interval|type</t>
-  </si>
-  <si>
-    <t>variation|location|interval|start|type</t>
-  </si>
-  <si>
-    <t>variation|location|interval|start|min</t>
-  </si>
-  <si>
-    <t>variation|location|interval|start|max</t>
-  </si>
-  <si>
-    <t>variation|location|interval|start|value</t>
-  </si>
-  <si>
-    <t>variation|location|interval|start|comparator</t>
-  </si>
-  <si>
-    <t>variation|location|interval|end|type</t>
-  </si>
-  <si>
-    <t>variation|location|interval|end|min</t>
-  </si>
-  <si>
-    <t>variation|location|interval|end|max</t>
-  </si>
-  <si>
-    <t>variation|location|interval|end|value</t>
-  </si>
-  <si>
-    <t>variation|location|interval|end|comparator</t>
-  </si>
-  <si>
-    <t>variation|location|interval|start</t>
-  </si>
-  <si>
-    <t>variation|location|interval|end</t>
-  </si>
-  <si>
     <t>variation|referenceBases</t>
   </si>
   <si>
@@ -1250,6 +1250,12 @@
   </si>
   <si>
     <t>runDate</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1286,12 +1292,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1299,6 +1299,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1315,13 +1327,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2616,10 +2629,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:EH1"/>
+  <dimension ref="A1:EH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BX1" sqref="BX1"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BN2" sqref="BN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2811,40 +2824,40 @@
       <c r="BJ1" t="s">
         <v>353</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BK1" t="s">
         <v>354</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BL1" t="s">
         <v>355</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BM1" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BN1" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BO1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="BP1" s="5" t="s">
+      <c r="BP1" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+      <c r="BQ1" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BR1" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BS1" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BU1" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BV1" s="5" t="s">
         <v>365</v>
       </c>
       <c r="BW1" t="s">
@@ -3038,6 +3051,14 @@
       </c>
       <c r="EH1" t="s">
         <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:138" x14ac:dyDescent="0.2">
+      <c r="BN2" t="s">
+        <v>408</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>